<commit_message>
finished part 3 of assign7 (basic part). I will run larger raytrace to produce image with higher quality
</commit_message>
<xml_diff>
--- a/assign7-results/assignment7_spreadsheet.xlsx
+++ b/assign7-results/assignment7_spreadsheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinhe7/Dropbox/Stanford Academic/CS148/HW/CS148-RT/cs148raytracer/cs148raytracer-public/assign7-results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinhe7/Dropbox/Stanford Academic/CS148/HW/CS148-RT/cs148raytracer/CS148-raytracer/assign7-results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="16420" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="16420" windowHeight="16600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>part 1</t>
   </si>
@@ -78,6 +78,30 @@
   </si>
   <si>
     <t>takeaway</t>
+  </si>
+  <si>
+    <t>part 3</t>
+  </si>
+  <si>
+    <t>grid size</t>
+  </si>
+  <si>
+    <t>samples/pixel</t>
+  </si>
+  <si>
+    <t>max reflection bounces</t>
+  </si>
+  <si>
+    <t>max refraction bounces</t>
+  </si>
+  <si>
+    <t>resolution</t>
+  </si>
+  <si>
+    <t>640 by 480</t>
+  </si>
+  <si>
+    <t>**basic</t>
   </si>
 </sst>
 </file>
@@ -392,13 +416,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J19"/>
+  <dimension ref="B2:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="135" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
@@ -565,7 +594,7 @@
         <v>1474031</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C17">
         <v>3</v>
       </c>
@@ -582,12 +611,60 @@
         <v>1474031</v>
       </c>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>16</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>11.55</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished large ray tracing
</commit_message>
<xml_diff>
--- a/assign7-results/assignment7_spreadsheet.xlsx
+++ b/assign7-results/assignment7_spreadsheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>part 1</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>**basic</t>
+  </si>
+  <si>
+    <t>960 by 720</t>
+  </si>
+  <si>
+    <t>**advanced</t>
   </si>
 </sst>
 </file>
@@ -416,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J25"/>
+  <dimension ref="B2:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="135" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -625,9 +631,6 @@
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>24</v>
-      </c>
       <c r="D24" t="s">
         <v>7</v>
       </c>
@@ -648,6 +651,9 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
       <c r="D25">
         <v>11.55</v>
       </c>
@@ -665,6 +671,29 @@
       </c>
       <c r="I25" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26">
+        <v>310.75</v>
+      </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
+      <c r="F26">
+        <v>16</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>8</v>
+      </c>
+      <c r="I26" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>